<commit_message>
Make Dipole work and begin to debug quads
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/Dipole.xlsx
+++ b/21-Spreads4Tests/Dipole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/00-Repository/lhara/LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D8AC78-EF69-EB47-8850-5F17FD72EF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A1782B-D263-9043-8CFB-CA6DB0628D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="12180" yWindow="640" windowWidth="18060" windowHeight="18720" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>MeV</t>
   </si>
@@ -47,23 +47,76 @@
     <t>Particle</t>
   </si>
   <si>
-    <t>Quad</t>
-  </si>
-  <si>
     <t>Length</t>
   </si>
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>k</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Rprime</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>1/c</t>
+  </si>
+  <si>
+    <t>s/m</t>
+  </si>
+  <si>
+    <t>1/c*10^9</t>
+  </si>
+  <si>
+    <t>Dipole test sheet:</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>radians</t>
+  </si>
+  <si>
+    <t>Dipole</t>
+  </si>
+  <si>
+    <t>Momentum</t>
   </si>
   <si>
     <r>
       <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MeV/c</t>
     </r>
     <r>
       <rPr>
@@ -72,68 +125,30 @@
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>-2</t>
+      <t>2</t>
     </r>
   </si>
   <si>
-    <t>sqrt(k)</t>
-  </si>
-  <si>
-    <r>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <t>l*sqrt(k)</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Rprime</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t>1/c</t>
-  </si>
-  <si>
-    <t>s/m</t>
-  </si>
-  <si>
-    <t>1/c*10^9</t>
-  </si>
-  <si>
-    <t>Dipole test sheet:</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>T</t>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>Tm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,6 +179,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -179,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -308,132 +337,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -449,9 +356,22 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="dotted">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -461,34 +381,15 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -513,21 +414,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,6 +443,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,26 +761,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E24" sqref="E24:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="A1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -880,234 +793,378 @@
       <c r="C2" s="12"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="18"/>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>0.25</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="12">
+      <c r="I4" s="12">
+        <v>938.27208815999995</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="16">
+        <f>E4/180*PI()</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="12">
         <v>299792458</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>1.4</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4">
-        <f>1/I3</f>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="13"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f>1/I5</f>
         <v>3.3356409519815204E-9</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D5" s="13"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="9">
-        <f>I4*1000000000</f>
-        <v>3.3356409519815204</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.2">
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="e">
-        <f>E4/B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>8</v>
+      <c r="J6" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="e">
-        <f>SQRT(E6)</f>
-        <v>#DIV/0!</v>
+        <v>20</v>
+      </c>
+      <c r="E7" s="30">
+        <f>SQRT((I4+B4)^2-I4^2)</f>
+        <v>194.75852619692921</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="9">
+        <f>I6*1000000000</f>
+        <v>3.3356409519815204</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="e">
-        <f>E7*E3</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="10"/>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D9" s="17"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="20"/>
+    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <f>E7*I7/1000</f>
+        <v>0.64964451573004278</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <f>B10/E3</f>
+        <v>1.2992890314600856</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f>B11*E5</f>
+        <v>1.0204592190312005</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="14" t="e">
-        <f>COS(E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="15" t="e">
-        <f>SIN(E8)/E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="17" t="e">
-        <f>-SIN(E8)*E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="18" t="e">
-        <f>COS(E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="18">
-        <v>0</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="17">
-        <v>0</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0</v>
-      </c>
-      <c r="D12" s="18" t="e">
-        <f>COSH(E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="19" t="e">
-        <f>SINH(E8)/E7</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>0</v>
-      </c>
-      <c r="C13" s="21">
-        <v>0</v>
-      </c>
-      <c r="D13" s="21" t="e">
-        <f>SINH(E8)*E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="22" t="e">
-        <f>COSH(E8)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="24">
+      <c r="B16" s="3">
+        <f>COS(E5)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B11*SIN(E5)</f>
+        <v>0.91873608486672786</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="23">
+        <f>B11*(1-COS(E5))</f>
+        <v>0.38055294659335753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
+        <f>-SIN(E5)/B11</f>
+        <v>-0.54422592977016904</v>
+      </c>
+      <c r="C17" s="10">
+        <f>COS(E5)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="24">
+        <f>SIN(E5)</f>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="13">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <f>B12</f>
+        <v>1.0204592190312005</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="13">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="21">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="13">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="23">
         <v>0.5</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="24" t="e">
-        <f t="array" ref="E15:E18">MMULT(B10:E13,B15:B18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="24" t="e">
-        <f>B$15*B10+B$16*C10+B$17*D10+B$18*E10</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="25">
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="23">
+        <f t="array" ref="E24:E29">MMULT(B16:G21,B24:B29)</f>
+        <v>0.46445464640961448</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="23">
+        <f>B$24*B16+B$25*C16+B$26*D16+B$27*E16+F$16*B28+G$16*B29</f>
+        <v>0.46445464640961448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="25">
         <v>0.1</v>
       </c>
-      <c r="E16" s="25" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="25" t="e">
-        <f t="shared" ref="H16:H17" si="0">B$15*B11+B$16*C11+B$17*D11+B$18*E11</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="25">
+      <c r="E25" s="25">
+        <v>-0.16604694770710238</v>
+      </c>
+      <c r="H25" s="25">
+        <f t="shared" ref="H25:H29" si="0">B$24*B17+B$25*C17+B$26*D17+B$27*E17+F$16*B29+G$16*B30</f>
+        <v>-0.20140228676642974</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="25">
         <v>-0.3</v>
       </c>
-      <c r="E17" s="25" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="25" t="e">
+      <c r="E26" s="25">
+        <v>-0.50409184380624006</v>
+      </c>
+      <c r="H26" s="25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="26">
+        <v>-0.50409184380624006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="25">
         <v>-0.2</v>
       </c>
-      <c r="E18" s="26" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="26" t="e">
-        <f>B$15*B13+B$16*C13+B$17*D13+B$18*E13</f>
-        <v>#DIV/0!</v>
+      <c r="E27" s="25">
+        <v>-0.2</v>
+      </c>
+      <c r="H27" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="25">
+        <v>0</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+      <c r="H28" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E29" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="H29" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Udate to focusquadrupole code, no update to documentation
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/Dipole.xlsx
+++ b/21-Spreads4Tests/Dipole.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ADC853-9F17-5747-8690-8686069F5924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F80D9F-FF15-D44C-AC7F-2BD670D02862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="19540" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="38640" yWindow="0" windowWidth="32780" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,8 +272,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -618,6 +618,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,23 +653,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,13 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,7 +979,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,14 +992,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -1019,23 +1012,23 @@
         <v>18</v>
       </c>
       <c r="F2" s="28"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="35"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="32">
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="34" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="1">
@@ -1054,14 +1047,14 @@
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="41">
-        <f>I13+B3</f>
+      <c r="B4" s="32">
+        <f>I10+B3</f>
         <v>958.27208815999995</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="34" t="s">
         <v>15</v>
       </c>
       <c r="E4">
@@ -1082,11 +1075,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="41">
-        <f>SQRT(B4^2 -I13^ 2)</f>
+      <c r="B5" s="32">
+        <f>SQRT(B4^2 -I10^ 2)</f>
         <v>194.75852619692921</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1112,11 +1105,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="33" t="s">
         <v>34</v>
       </c>
       <c r="B6">
-        <f>B5/I13</f>
+        <f>B5/I10</f>
         <v>0.20757148022900346</v>
       </c>
       <c r="C6" s="6"/>
@@ -1124,7 +1117,7 @@
         <v>23</v>
       </c>
       <c r="E6">
-        <f>B5*I16/1000</f>
+        <f>B5*I13/1000</f>
         <v>0.64964451573004278</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1134,7 +1127,7 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="33" t="s">
         <v>36</v>
       </c>
       <c r="B7">
@@ -1145,7 +1138,7 @@
       <c r="D7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="35">
         <f>E6/E3</f>
         <v>1.2992890314600856</v>
       </c>
@@ -1175,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="36" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="8">
@@ -1192,7 +1185,7 @@
         <v>28</v>
       </c>
       <c r="J8" s="9">
-        <f>B5*I16/J7/1000</f>
+        <f>B5*I13/J7/1000</f>
         <v>0.50000000000000011</v>
       </c>
       <c r="L8">
@@ -1201,28 +1194,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="37"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="44"/>
       <c r="C10" s="45"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="37"/>
+      <c r="D10" s="1"/>
+      <c r="H10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="11">
+        <v>938.27208815999995</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -1232,50 +1223,58 @@
         <f>B4+B5*B32</f>
         <v>968.0100144698464</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="37"/>
+      <c r="D11" s="1"/>
+      <c r="H11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="11">
+        <v>299792458</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="41">
-        <f>SQRT(B11^2 -I13^ 2)</f>
+      <c r="B12" s="32">
+        <f>SQRT(B11^2 -I10^ 2)</f>
         <v>238.09426010255984</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="H12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f>1/I11</f>
+        <v>3.3356409519815204E-9</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B13">
-        <f>B12*I16/1000</f>
+        <f>B12*I13/1000</f>
         <v>0.79419696442983845</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="H13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="11">
-        <v>938.27208815999995</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>20</v>
+      <c r="H13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8">
+        <f>I12*1000000000</f>
+        <v>3.3356409519815204</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1290,42 +1289,13 @@
         <v>4</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="H14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="11">
-        <v>299792458</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="D15" s="1"/>
-      <c r="H15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15">
-        <f>1/I14</f>
-        <v>3.3356409519815204E-9</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
-      <c r="H16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="8">
-        <f>I15*1000000000</f>
-        <v>3.3356409519815204</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D17" s="1"/>

</xml_diff>